<commit_message>
gas flux calc pt1
</commit_message>
<xml_diff>
--- a/04_Output/rC_k600.xlsx
+++ b/04_Output/rC_k600.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">logQ</t>
   </si>
@@ -46,10 +46,13 @@
     <t xml:space="preserve">Temp</t>
   </si>
   <si>
-    <t xml:space="preserve">KCO2_1d</t>
+    <t xml:space="preserve">KCO2_dh</t>
   </si>
   <si>
-    <t xml:space="preserve">k600_1d</t>
+    <t xml:space="preserve">k600_dh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KCO2_1d</t>
   </si>
   <si>
     <t xml:space="preserve">log_K600</t>
@@ -453,6 +456,9 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="e">
@@ -462,7 +468,7 @@
         <v>45442.6111111111</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
         <v>749.64344</v>
@@ -479,14 +485,17 @@
       <c r="H2" t="n">
         <v>73.38625</v>
       </c>
-      <c r="I2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K2" t="e">
-        <v>#NUM!</v>
+      <c r="I2" t="n">
+        <v>-0.00722301206835864</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.00677704959333723</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.00722301206835864</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-2.16895933625257</v>
       </c>
     </row>
     <row r="3">
@@ -497,7 +506,7 @@
         <v>45590.5591435185</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
         <v>380.7333</v>
@@ -514,14 +523,17 @@
       <c r="H3" t="n">
         <v>68.7704583333333</v>
       </c>
-      <c r="I3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K3" t="e">
-        <v>#NUM!</v>
+      <c r="I3" t="n">
+        <v>-0.0333313008490599</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0338039543046863</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0333313008490599</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1.47103249403429</v>
       </c>
     </row>
     <row r="4">
@@ -532,7 +544,7 @@
         <v>45639.6267361111</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
         <v>350.53264</v>
@@ -549,25 +561,28 @@
       <c r="H4" t="n">
         <v>56.3528333333333</v>
       </c>
-      <c r="I4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K4" t="e">
-        <v>#NUM!</v>
+      <c r="I4" t="n">
+        <v>-0.187318140691708</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.237662875388165</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.187318140691708</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.624038652824875</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.499025265749003</v>
+        <v>0.499025265741148</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45331.5462962963</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" t="n">
         <v>841.7328192</v>
@@ -579,19 +594,22 @@
         <v>0.0534585500989185</v>
       </c>
       <c r="G5" t="n">
-        <v>3.15518817595706</v>
+        <v>3.1551881759</v>
       </c>
       <c r="H5" t="n">
         <v>58.7118333333333</v>
       </c>
       <c r="I5" t="n">
-        <v>2442.33913134876</v>
+        <v>5.44016286715653</v>
       </c>
       <c r="J5" t="n">
-        <v>2965.2972577307</v>
+        <v>6.60502050044093</v>
       </c>
       <c r="K5" t="n">
-        <v>3.47206823595364</v>
+        <v>5.44016286715653</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.819874169901274</v>
       </c>
     </row>
     <row r="6">
@@ -602,7 +620,7 @@
         <v>45569.5924768519</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="n">
         <v>410.829216</v>
@@ -619,25 +637,28 @@
       <c r="H6" t="n">
         <v>75.485125</v>
       </c>
-      <c r="I6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K6" t="e">
-        <v>#NUM!</v>
+      <c r="I6" t="n">
+        <v>-0.0273600587330568</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.0247946706179097</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.0273600587330568</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1.6056416566721</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.129645221247688</v>
+        <v>0.129645221267409</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>45231.64375</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" t="n">
         <v>861.608416666667</v>
@@ -649,30 +670,33 @@
         <v>0.0367414206545583</v>
       </c>
       <c r="G7" t="n">
-        <v>1.34786135364712</v>
+        <v>1.34786135370833</v>
       </c>
       <c r="H7" t="n">
         <v>68.2418333333333</v>
       </c>
       <c r="I7" t="n">
-        <v>15.2165979978598</v>
+        <v>-0.0232949761654448</v>
       </c>
       <c r="J7" t="n">
-        <v>15.5766160020993</v>
+        <v>0.023846125037819</v>
       </c>
       <c r="K7" t="n">
-        <v>1.19247311371887</v>
+        <v>0.0232949761654448</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-1.62258218314034</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.30080534455042</v>
+        <v>2.30080534454963</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>45279.6388888889</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" t="n">
         <v>682.46505</v>
@@ -684,19 +708,22 @@
         <v>0.335585069806503</v>
       </c>
       <c r="G8" t="n">
-        <v>199.896571092031</v>
+        <v>199.896571091667</v>
       </c>
       <c r="H8" t="n">
         <v>58.1367916666667</v>
       </c>
       <c r="I8" t="n">
-        <v>2.42642112532325</v>
+        <v>-0.0339279459467323</v>
       </c>
       <c r="J8" t="n">
-        <v>2.97765244901289</v>
+        <v>0.0416356543733956</v>
       </c>
       <c r="K8" t="n">
-        <v>0.473874005610801</v>
+        <v>0.0339279459467323</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1.38053460529363</v>
       </c>
     </row>
   </sheetData>
@@ -747,16 +774,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.4881172315497</v>
+        <v>1.48811723155117</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45296.4760416667</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
         <v>638.458466666667</v>
@@ -768,30 +798,33 @@
         <v>0.215852248068133</v>
       </c>
       <c r="G2" t="n">
-        <v>30.7692727491814</v>
+        <v>30.7692727492857</v>
       </c>
       <c r="H2" t="n">
         <v>53.7677083333333</v>
       </c>
       <c r="I2" t="n">
-        <v>5.22892126526682</v>
+        <v>-0.0470281004199628</v>
       </c>
       <c r="J2" t="n">
-        <v>6.9677990541449</v>
+        <v>0.0626672954135077</v>
       </c>
       <c r="K2" t="n">
-        <v>0.843095617468262</v>
+        <v>0.0470281004199628</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1.20295904811693</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.97546997200686</v>
+        <v>1.97546997200062</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45684.4790509259</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="n">
         <v>351.12894</v>
@@ -803,30 +836,33 @@
         <v>0.297576481764534</v>
       </c>
       <c r="G3" t="n">
-        <v>94.5083045240855</v>
+        <v>94.5083045227273</v>
       </c>
       <c r="H3" t="n">
         <v>51.2003333333333</v>
       </c>
       <c r="I3" t="n">
-        <v>29.9809396779035</v>
+        <v>-0.371734272889384</v>
       </c>
       <c r="J3" t="n">
-        <v>41.9548094541104</v>
+        <v>0.520198524602315</v>
       </c>
       <c r="K3" t="n">
-        <v>1.62278175299922</v>
+        <v>0.371734272889384</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-0.283830883893283</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.6248134307019</v>
+        <v>1.62481343070708</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45484.5087962963</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="n">
         <v>792.3951</v>
@@ -838,30 +874,33 @@
         <v>0.236097905442564</v>
       </c>
       <c r="G4" t="n">
-        <v>42.1515385023547</v>
+        <v>42.1515385028571</v>
       </c>
       <c r="H4" t="n">
         <v>76.44125</v>
       </c>
       <c r="I4" t="n">
-        <v>37.9449411668583</v>
+        <v>-0.373280047151523</v>
       </c>
       <c r="J4" t="n">
-        <v>33.8550834326527</v>
+        <v>0.333046428626357</v>
       </c>
       <c r="K4" t="n">
-        <v>1.52962388841246</v>
+        <v>0.373280047151523</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.477495219074176</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.06577306541398</v>
+        <v>1.06577306544163</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45590.4100694444</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
         <v>546.66366</v>
@@ -873,30 +912,33 @@
         <v>0.163249695310579</v>
       </c>
       <c r="G5" t="n">
-        <v>11.6351789032592</v>
+        <v>11.635178904</v>
       </c>
       <c r="H5" t="n">
         <v>69.3495</v>
       </c>
       <c r="I5" t="n">
-        <v>133.147923773774</v>
+        <v>0.905681582804368</v>
       </c>
       <c r="J5" t="n">
-        <v>133.708572612851</v>
+        <v>0.909495155810849</v>
       </c>
       <c r="K5" t="n">
-        <v>2.12615925258064</v>
+        <v>0.905681582804368</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-0.0411996097508221</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.3246951004139</v>
+        <v>0.32469510041924</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45639.4833333333</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="n">
         <v>660.91974</v>
@@ -908,30 +950,33 @@
         <v>0.100274044883754</v>
       </c>
       <c r="G6" t="n">
-        <v>2.11200577028172</v>
+        <v>2.11200577030769</v>
       </c>
       <c r="H6" t="n">
         <v>55.5208333333333</v>
       </c>
       <c r="I6" t="n">
-        <v>81.783855367662</v>
+        <v>-0.341699915995974</v>
       </c>
       <c r="J6" t="n">
-        <v>105.395844870759</v>
+        <v>0.440352819963818</v>
       </c>
       <c r="K6" t="n">
-        <v>2.02282348957414</v>
+        <v>0.341699915995974</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.356199218144873</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.84742212067015</v>
+        <v>2.84742212066537</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>45279.4587962963</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="n">
         <v>743.7952</v>
@@ -943,30 +988,33 @@
         <v>0.528260069853473</v>
       </c>
       <c r="G7" t="n">
-        <v>703.756016428581</v>
+        <v>703.756016420833</v>
       </c>
       <c r="H7" t="n">
         <v>57.950125</v>
       </c>
       <c r="I7" t="n">
-        <v>24.5945005502199</v>
+        <v>-0.541345524111269</v>
       </c>
       <c r="J7" t="n">
-        <v>30.2831430737235</v>
+        <v>0.666557303146162</v>
       </c>
       <c r="K7" t="n">
-        <v>1.48120094839522</v>
+        <v>0.541345524111269</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.176162508860153</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.04776300348103</v>
+        <v>2.04776300345066</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>45502.4672453704</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
         <v>801.7695</v>
@@ -978,30 +1026,33 @@
         <v>0.312017862477283</v>
       </c>
       <c r="G8" t="n">
-        <v>111.625393657806</v>
+        <v>111.62539365</v>
       </c>
       <c r="H8" t="n">
         <v>76.3831666666667</v>
       </c>
       <c r="I8" t="n">
-        <v>106.921669755234</v>
+        <v>1.39006128539709</v>
       </c>
       <c r="J8" t="n">
-        <v>95.4812610289166</v>
+        <v>1.24132745720325</v>
       </c>
       <c r="K8" t="n">
-        <v>1.97991814613576</v>
+        <v>1.39006128539709</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.093886361754324</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.71108095362448</v>
+        <v>1.71108095362215</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>45569.4208333333</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" t="n">
         <v>693.87467</v>
@@ -1013,19 +1064,22 @@
         <v>0.249963155450786</v>
       </c>
       <c r="G9" t="n">
-        <v>51.4139479591211</v>
+        <v>51.4139479588462</v>
       </c>
       <c r="H9" t="n">
         <v>76.3036666666667</v>
       </c>
       <c r="I9" t="n">
-        <v>262.116599005408</v>
+        <v>-2.72997884097584</v>
       </c>
       <c r="J9" t="n">
-        <v>234.414519987693</v>
+        <v>2.44145804581688</v>
       </c>
       <c r="K9" t="n">
-        <v>2.36998450903218</v>
+        <v>2.72997884097584</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.387649265737992</v>
       </c>
     </row>
   </sheetData>
@@ -1076,16 +1130,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.5793165496351</v>
+        <v>1.5793165496371</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45296.6100694444</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
         <v>456.123866666667</v>
@@ -1097,30 +1154,33 @@
         <v>0.412753905123254</v>
       </c>
       <c r="G2" t="n">
-        <v>37.9591561800967</v>
+        <v>37.9591561802707</v>
       </c>
       <c r="H2" t="n">
         <v>54.8325956006768</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0708810643150279</v>
+        <v>-0.00121901817063835</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0925662232043585</v>
+        <v>0.00159196125458791</v>
       </c>
       <c r="K2" t="n">
-        <v>-1.03354745556387</v>
+        <v>0.00121901817063835</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-2.7980675063995</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.87100816824727</v>
+        <v>1.87100816824501</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45684.528587963</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="n">
         <v>329.190888</v>
@@ -1132,30 +1192,33 @@
         <v>0.514586113304458</v>
       </c>
       <c r="G3" t="n">
-        <v>74.3033112794777</v>
+        <v>74.3033112790909</v>
       </c>
       <c r="H3" t="n">
         <v>51.4724285714286</v>
       </c>
       <c r="I3" t="n">
-        <v>0.686889621673731</v>
+        <v>-0.0147276608619273</v>
       </c>
       <c r="J3" t="n">
-        <v>0.956243105494021</v>
+        <v>0.0205028926262647</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0194316830871586</v>
+        <v>0.0147276608619273</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1.68818486270022</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.37477885123213</v>
+        <v>1.37477885121376</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45590.4736111111</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
         <v>411.06708</v>
@@ -1167,30 +1230,33 @@
         <v>0.353585946262801</v>
       </c>
       <c r="G4" t="n">
-        <v>23.7016647670735</v>
+        <v>23.7016647660714</v>
       </c>
       <c r="H4" t="n">
         <v>68.4775833333333</v>
       </c>
       <c r="I4" t="n">
-        <v>2.09988598413225</v>
+        <v>-0.0309370905309748</v>
       </c>
       <c r="J4" t="n">
-        <v>2.14024553622096</v>
+        <v>0.0315316976316427</v>
       </c>
       <c r="K4" t="n">
-        <v>0.330463599942121</v>
+        <v>0.0309370905309748</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1.50125264668922</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.25618350175535</v>
+        <v>1.25618350175115</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45231.5059027778</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
         <v>714.0472</v>
@@ -1202,19 +1268,22 @@
         <v>0.323240054140384</v>
       </c>
       <c r="G5" t="n">
-        <v>18.037797280416</v>
+        <v>18.0377972802419</v>
       </c>
       <c r="H5" t="n">
         <v>67.2085132275132</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0727481208053596</v>
+        <v>-0.000979796104488986</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0758058207694044</v>
+        <v>0.00102097823373577</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.12029744567433</v>
+        <v>0.000979796104488986</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-2.9909835165509</v>
       </c>
     </row>
     <row r="6">
@@ -1225,7 +1294,7 @@
         <v>45639.5269675926</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
         <v>365.8083</v>
@@ -1242,25 +1311,28 @@
       <c r="H6" t="n">
         <v>54.87</v>
       </c>
-      <c r="I6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K6" t="e">
-        <v>#NUM!</v>
+      <c r="I6" t="n">
+        <v>-0.116594826346693</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.152109837643059</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.116594826346693</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.817842697216342</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.56499734138787</v>
+        <v>2.56499734139219</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>45279.4587962963</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="n">
         <v>743.7952</v>
@@ -1272,30 +1344,33 @@
         <v>0.868715799079058</v>
       </c>
       <c r="G7" t="n">
-        <v>367.280052120008</v>
+        <v>367.280052123662</v>
       </c>
       <c r="H7" t="n">
         <v>58.6289981220657</v>
       </c>
       <c r="I7" t="n">
-        <v>4.54457774345002</v>
+        <v>-0.16449777024492</v>
       </c>
       <c r="J7" t="n">
-        <v>5.52688689568124</v>
+        <v>0.200053915250054</v>
       </c>
       <c r="K7" t="n">
-        <v>0.742480577105002</v>
+        <v>0.16449777024492</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.698852944635622</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.48789393781438</v>
+        <v>1.48789393782397</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>45569.462962963</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
         <v>395.82372</v>
@@ -1307,19 +1382,22 @@
         <v>0.385103328321135</v>
       </c>
       <c r="G8" t="n">
-        <v>30.7534567069137</v>
+        <v>30.7534567075926</v>
       </c>
       <c r="H8" t="n">
         <v>75.4362222222222</v>
       </c>
       <c r="I8" t="n">
-        <v>14.7748394060531</v>
+        <v>-0.23707665961172</v>
       </c>
       <c r="J8" t="n">
-        <v>13.4013452642964</v>
+        <v>0.215037611052551</v>
       </c>
       <c r="K8" t="n">
-        <v>1.12714839624061</v>
+        <v>0.23707665961172</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-0.667485573367981</v>
       </c>
     </row>
   </sheetData>
@@ -1370,16 +1448,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.468650986440939</v>
+        <v>0.468650986424036</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45660.4115740741</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="n">
         <v>552.81112</v>
@@ -1391,30 +1472,33 @@
         <v>0.00525665233148642</v>
       </c>
       <c r="G2" t="n">
-        <v>2.9420563487145</v>
+        <v>2.9420563486</v>
       </c>
       <c r="H2" t="n">
         <v>58.6762916666667</v>
       </c>
       <c r="I2" t="n">
-        <v>3161.70241227499</v>
+        <v>-0.692498764872981</v>
       </c>
       <c r="J2" t="n">
-        <v>3841.25482029939</v>
+        <v>0.841339212790009</v>
       </c>
       <c r="K2" t="n">
-        <v>3.5844731182506</v>
+        <v>0.692498764872981</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.0750288691951065</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.05743043314321</v>
+        <v>2.05743043317364</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45684.409837963</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" t="n">
         <v>560.080524</v>
@@ -1426,19 +1510,22 @@
         <v>0.161457401795922</v>
       </c>
       <c r="G3" t="n">
-        <v>114.13804595354</v>
+        <v>114.138045961538</v>
       </c>
       <c r="H3" t="n">
         <v>53.0998181818182</v>
       </c>
       <c r="I3" t="n">
-        <v>24.1248106339086</v>
+        <v>-0.16229705182373</v>
       </c>
       <c r="J3" t="n">
-        <v>32.5584369350977</v>
+        <v>0.21903335975322</v>
       </c>
       <c r="K3" t="n">
-        <v>1.51266354711531</v>
+        <v>0.16229705182373</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-0.65948973514438</v>
       </c>
     </row>
     <row r="4">
@@ -1449,7 +1536,7 @@
         <v>45442.334837963</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
         <v>892.5125</v>
@@ -1466,25 +1553,28 @@
       <c r="H4" t="n">
         <v>72.257625</v>
       </c>
-      <c r="I4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K4" t="e">
-        <v>#NUM!</v>
+      <c r="I4" t="n">
+        <v>-0.0323566680786453</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.0309288241918769</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.0323566680786453</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1.50963659007396</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2.2728374417132</v>
+        <v>2.27283744171538</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45484.4175925926</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
         <v>2034.862788</v>
@@ -1496,30 +1586,33 @@
         <v>0.25670942796431</v>
       </c>
       <c r="G5" t="n">
-        <v>187.429282091365</v>
+        <v>187.429282092308</v>
       </c>
       <c r="H5" t="n">
         <v>76.5790416666667</v>
       </c>
       <c r="I5" t="n">
-        <v>5.23630994528206</v>
+        <v>-0.0560087554457162</v>
       </c>
       <c r="J5" t="n">
-        <v>4.66096747896893</v>
+        <v>0.0498547623035987</v>
       </c>
       <c r="K5" t="n">
-        <v>0.668476072734428</v>
+        <v>0.0560087554457162</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1.30229335002258</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.11979583477163</v>
+        <v>0.00826695036340704</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45590.3521990741</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="n">
         <v>551.097192</v>
@@ -1531,19 +1624,22 @@
         <v>0.00145530175357868</v>
       </c>
       <c r="G6" t="n">
-        <v>0.758934272109195</v>
+        <v>1.019217684125</v>
       </c>
       <c r="H6" t="n">
         <v>69.5068333333333</v>
       </c>
       <c r="I6" t="n">
-        <v>338.844350300782</v>
+        <v>-0.0205466990492898</v>
       </c>
       <c r="J6" t="n">
-        <v>339.329787940342</v>
+        <v>0.0205761348096275</v>
       </c>
       <c r="K6" t="n">
-        <v>2.53062198569958</v>
+        <v>0.0205466990492898</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1.68663620335902</v>
       </c>
     </row>
     <row r="7">
@@ -1554,7 +1650,7 @@
         <v>45597.3579861111</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
         <v>628.45452</v>
@@ -1571,25 +1667,28 @@
       <c r="H7" t="n">
         <v>69.6570416666667</v>
       </c>
-      <c r="I7" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J7" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K7" t="e">
-        <v>#NUM!</v>
+      <c r="I7" t="n">
+        <v>1.64331633910974</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.64162808869427</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.64331633910974</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.215274774389667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.21153465609192</v>
+        <v>2.21153465604911</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>45296.4006944444</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
         <v>426.60745</v>
@@ -1601,19 +1700,22 @@
         <v>0.225012367816944</v>
       </c>
       <c r="G8" t="n">
-        <v>162.755118676755</v>
+        <v>162.755118660714</v>
       </c>
       <c r="H8" t="n">
         <v>54.8710416666667</v>
       </c>
       <c r="I8" t="n">
-        <v>4.60331475600706</v>
+        <v>-0.0431584480439927</v>
       </c>
       <c r="J8" t="n">
-        <v>6.00549340048817</v>
+        <v>0.056304595414703</v>
       </c>
       <c r="K8" t="n">
-        <v>0.778548694054773</v>
+        <v>0.0431584480439927</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1.24945615786977</v>
       </c>
     </row>
     <row r="9">
@@ -1624,7 +1726,7 @@
         <v>45618.3987268519</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" t="n">
         <v>3118.512384</v>
@@ -1641,25 +1743,28 @@
       <c r="H9" t="n">
         <v>62.832875</v>
       </c>
-      <c r="I9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J9" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K9" t="e">
-        <v>#NUM!</v>
+      <c r="I9" t="n">
+        <v>0.563667320801013</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.634680597323982</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.563667320801013</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-0.197444778200821</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.99360035723806</v>
+        <v>1.99360035726142</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>45266.452662037</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n">
         <v>409.7124</v>
@@ -1671,19 +1776,22 @@
         <v>0.140716626048637</v>
       </c>
       <c r="G10" t="n">
-        <v>98.5372317396999</v>
+        <v>98.537231745</v>
       </c>
       <c r="H10" t="n">
         <v>62.9686666666667</v>
       </c>
       <c r="I10" t="n">
-        <v>5.75876431979859</v>
+        <v>-0.0337647452204721</v>
       </c>
       <c r="J10" t="n">
-        <v>6.46958238000064</v>
+        <v>0.0379324085190583</v>
       </c>
       <c r="K10" t="n">
-        <v>0.81087624729699</v>
+        <v>0.0337647452204721</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-1.42098958088467</v>
       </c>
     </row>
     <row r="11">
@@ -1694,7 +1802,7 @@
         <v>45635.3928240741</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" t="n">
         <v>2329.16652</v>
@@ -1711,25 +1819,28 @@
       <c r="H11" t="n">
         <v>56.8723333333333</v>
       </c>
-      <c r="I11" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J11" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K11" t="e">
-        <v>#NUM!</v>
+      <c r="I11" t="n">
+        <v>2.152726136449</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2.70467538288039</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.152726136449</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.432115148228664</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2.73623324833003</v>
+        <v>2.73623324833723</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>45279.4179398148</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
         <v>444.28</v>
@@ -1741,30 +1852,33 @@
         <v>0.69658739105357</v>
       </c>
       <c r="G12" t="n">
-        <v>544.795169674302</v>
+        <v>544.795169683333</v>
       </c>
       <c r="H12" t="n">
         <v>59.3927083333333</v>
       </c>
       <c r="I12" t="n">
-        <v>1.92361508691423</v>
+        <v>-0.0558319172827028</v>
       </c>
       <c r="J12" t="n">
-        <v>2.30614023018154</v>
+        <v>0.0669345085977433</v>
       </c>
       <c r="K12" t="n">
-        <v>0.362885712040372</v>
+        <v>0.0558319172827028</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-1.17434992065355</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2.49799189071829</v>
+        <v>2.49799189070893</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>45502.4107638889</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" t="n">
         <v>1722.98714</v>
@@ -1776,30 +1890,33 @@
         <v>0.416947772916525</v>
       </c>
       <c r="G13" t="n">
-        <v>314.768953891403</v>
+        <v>314.768953884615</v>
       </c>
       <c r="H13" t="n">
         <v>76.3617916666667</v>
       </c>
       <c r="I13" t="n">
-        <v>1.51139246729725</v>
+        <v>-0.0262571551350999</v>
       </c>
       <c r="J13" t="n">
-        <v>1.35007271120727</v>
+        <v>0.023454575425552</v>
       </c>
       <c r="K13" t="n">
-        <v>0.130357159032578</v>
+        <v>0.0262571551350999</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-1.62977242423926</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.6697577409753</v>
+        <v>1.66975774097199</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>45569.3364583333</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
         <v>520.154188</v>
@@ -1811,19 +1928,22 @@
         <v>0.0700180580780742</v>
       </c>
       <c r="G14" t="n">
-        <v>46.747430108433</v>
+        <v>46.7474301080769</v>
       </c>
       <c r="H14" t="n">
         <v>75.6006666666667</v>
       </c>
       <c r="I14" t="n">
-        <v>1.9735868782611</v>
+        <v>-0.00575778002767546</v>
       </c>
       <c r="J14" t="n">
-        <v>1.78537435630409</v>
+        <v>0.00520868522378351</v>
       </c>
       <c r="K14" t="n">
-        <v>0.251729292622446</v>
+        <v>0.00575778002767546</v>
+      </c>
+      <c r="L14" t="n">
+        <v>-2.28327188747123</v>
       </c>
     </row>
   </sheetData>
@@ -1874,16 +1994,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.15052348266254</v>
+        <v>1.15052348266631</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45296.4349537037</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
         <v>618.29095</v>
@@ -1895,30 +2018,33 @@
         <v>0.425990517738611</v>
       </c>
       <c r="G2" t="n">
-        <v>14.1424119219607</v>
+        <v>14.1424119220833</v>
       </c>
       <c r="H2" t="n">
         <v>55.2622916666667</v>
       </c>
       <c r="I2" t="n">
-        <v>1.2851116692374</v>
+        <v>-0.0228102243887654</v>
       </c>
       <c r="J2" t="n">
-        <v>1.66460884481262</v>
+        <v>0.0295461493180833</v>
       </c>
       <c r="K2" t="n">
-        <v>0.221312197904229</v>
+        <v>0.0228102243887654</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1.52949911169909</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.1415133928052</v>
+        <v>1.14151339272529</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45684.4493055556</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="n">
         <v>438.31809</v>
@@ -1930,30 +2056,33 @@
         <v>0.423142070899526</v>
       </c>
       <c r="G3" t="n">
-        <v>13.8520290225487</v>
+        <v>13.85202902</v>
       </c>
       <c r="H3" t="n">
         <v>52.7025454545455</v>
       </c>
       <c r="I3" t="n">
-        <v>11.1455271474515</v>
+        <v>-0.196505893268312</v>
       </c>
       <c r="J3" t="n">
-        <v>15.1561061813325</v>
+        <v>0.26721608984759</v>
       </c>
       <c r="K3" t="n">
-        <v>1.18058763921349</v>
+        <v>0.196505893268312</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-0.573137395292139</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.888330297949479</v>
+        <v>0.888330297947025</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45590.3826388889</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="n">
         <v>921.7171</v>
@@ -1965,30 +2094,33 @@
         <v>0.350465352119515</v>
       </c>
       <c r="G4" t="n">
-        <v>7.73268462442831</v>
+        <v>7.73268462438462</v>
       </c>
       <c r="H4" t="n">
         <v>68.2630833333333</v>
       </c>
       <c r="I4" t="n">
-        <v>42.888077344184</v>
+        <v>-0.626282713673269</v>
       </c>
       <c r="J4" t="n">
-        <v>43.8755145968776</v>
+        <v>0.640701986359151</v>
       </c>
       <c r="K4" t="n">
-        <v>1.64222222315533</v>
+        <v>0.626282713673269</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.193343929569118</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.937225889387457</v>
+        <v>0.937225889386442</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45231.4138888889</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="n">
         <v>434.69795</v>
@@ -2000,30 +2132,33 @@
         <v>0.36326953896332</v>
       </c>
       <c r="G5" t="n">
-        <v>8.65417931160357</v>
+        <v>8.65417931158333</v>
       </c>
       <c r="H5" t="n">
         <v>67.2998333333333</v>
       </c>
       <c r="I5" t="n">
-        <v>0.80706235080412</v>
+        <v>-0.0122158820038028</v>
       </c>
       <c r="J5" t="n">
-        <v>0.839668088680685</v>
+        <v>0.0127094099773852</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0758923517245445</v>
+        <v>0.0122158820038028</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1.89587461069805</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.02138493772845</v>
+        <v>1.02138493779272</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45569.4001157407</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="n">
         <v>555.11052</v>
@@ -2035,19 +2170,22 @@
         <v>0.386909393539067</v>
       </c>
       <c r="G6" t="n">
-        <v>10.5047310494453</v>
+        <v>10.504731051</v>
       </c>
       <c r="H6" t="n">
         <v>75.3191666666667</v>
       </c>
       <c r="I6" t="n">
-        <v>7.83767603189423</v>
+        <v>-0.126352936677328</v>
       </c>
       <c r="J6" t="n">
-        <v>7.12167092180563</v>
+        <v>0.114810057389193</v>
       </c>
       <c r="K6" t="n">
-        <v>0.85258190192096</v>
+        <v>0.126352936677328</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.940020065968447</v>
       </c>
     </row>
   </sheetData>
@@ -2098,6 +2236,9 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="e">
@@ -2107,7 +2248,7 @@
         <v>45660.5268518519</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="n">
         <v>350.63274</v>
@@ -2124,25 +2265,28 @@
       <c r="H2" t="n">
         <v>60.6108333333333</v>
       </c>
-      <c r="I2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K2" t="e">
-        <v>#NUM!</v>
+      <c r="I2" t="n">
+        <v>-0.0457362341132933</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0536290117969964</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0457362341132933</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1.2706002055554</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.13331324235291</v>
+        <v>2.13331324234938</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45296.6502314815</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
         <v>612.310275</v>
@@ -2154,30 +2298,33 @@
         <v>0.287726779544469</v>
       </c>
       <c r="G3" t="n">
-        <v>135.929350688605</v>
+        <v>135.9293506875</v>
       </c>
       <c r="H3" t="n">
         <v>57.3474166666667</v>
       </c>
       <c r="I3" t="n">
-        <v>2.29763769799997</v>
+        <v>-0.0275454956418957</v>
       </c>
       <c r="J3" t="n">
-        <v>2.86156511357376</v>
+        <v>0.0343062047743908</v>
       </c>
       <c r="K3" t="n">
-        <v>0.456603632524347</v>
+        <v>0.0275454956418957</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1.46462732440105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.0235293889573</v>
+        <v>2.02352938896741</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45684.5840277778</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
         <v>345.56298</v>
@@ -2189,19 +2336,22 @@
         <v>0.239089827931722</v>
       </c>
       <c r="G4" t="n">
-        <v>105.567293879362</v>
+        <v>105.567293881818</v>
       </c>
       <c r="H4" t="n">
         <v>52.6218666666667</v>
       </c>
       <c r="I4" t="n">
-        <v>1.4288656991903</v>
+        <v>-0.0142344689232062</v>
       </c>
       <c r="J4" t="n">
-        <v>1.94570380717799</v>
+        <v>0.0193832495193451</v>
       </c>
       <c r="K4" t="n">
-        <v>0.289076728687383</v>
+        <v>0.0142344689232062</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1.71257341355879</v>
       </c>
     </row>
     <row r="5">
@@ -2212,7 +2362,7 @@
         <v>45442.5159722222</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="n">
         <v>664.4421</v>
@@ -2229,25 +2379,28 @@
       <c r="H5" t="n">
         <v>69.957</v>
       </c>
-      <c r="I5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K5" t="e">
-        <v>#NUM!</v>
+      <c r="I5" t="n">
+        <v>-0.0120268373437539</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.0119519645480923</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0120268373437539</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1.92256070373071</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.998833642320927</v>
+        <v>-0.566360259554675</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45484.5509259259</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="n">
         <v>20118.9135</v>
@@ -2259,30 +2412,33 @@
         <v>0.0013654681854821</v>
       </c>
       <c r="G6" t="n">
-        <v>0.100268924736074</v>
+        <v>0.271418684</v>
       </c>
       <c r="H6" t="n">
         <v>73.537</v>
       </c>
       <c r="I6" t="n">
-        <v>32458.750221616</v>
+        <v>1.84672461533862</v>
       </c>
       <c r="J6" t="n">
-        <v>30372.9383772734</v>
+        <v>1.72805337724063</v>
       </c>
       <c r="K6" t="n">
-        <v>4.48248680901756</v>
+        <v>1.84672461533862</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.237557153121486</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.9468491266343</v>
+        <v>1.94684912663333</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>45590.5094907407</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
         <v>509.79309</v>
@@ -2294,30 +2450,33 @@
         <v>0.210021357525233</v>
       </c>
       <c r="G7" t="n">
-        <v>88.4808175167356</v>
+        <v>88.4808175165385</v>
       </c>
       <c r="H7" t="n">
         <v>68.8635</v>
       </c>
       <c r="I7" t="n">
-        <v>22.2991493012617</v>
+        <v>-0.195137400329535</v>
       </c>
       <c r="J7" t="n">
-        <v>22.5804118145796</v>
+        <v>0.1975986976157</v>
       </c>
       <c r="K7" t="n">
-        <v>1.35373185818986</v>
+        <v>0.195137400329535</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.704215922198688</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.70660519514956</v>
+        <v>1.70660519515198</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>45597.4420138889</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
         <v>709.2594</v>
@@ -2329,30 +2488,33 @@
         <v>0.140018529582514</v>
       </c>
       <c r="G8" t="n">
-        <v>50.886806313883</v>
+        <v>50.8868063141667</v>
       </c>
       <c r="H8" t="n">
         <v>69.1992916666667</v>
       </c>
       <c r="I8" t="n">
-        <v>421.436718042855</v>
+        <v>-2.45870623218505</v>
       </c>
       <c r="J8" t="n">
-        <v>424.255976125793</v>
+        <v>2.47515408098865</v>
       </c>
       <c r="K8" t="n">
-        <v>2.62762796856231</v>
+        <v>2.45870623218505</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.393602239407076</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.782366260768942</v>
+        <v>0.782366260755101</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>45618.5153935185</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
         <v>2030.428296</v>
@@ -2364,30 +2526,33 @@
         <v>0.02724196474367</v>
       </c>
       <c r="G9" t="n">
-        <v>6.05851602244309</v>
+        <v>6.05851602225</v>
       </c>
       <c r="H9" t="n">
         <v>65.92275</v>
       </c>
       <c r="I9" t="n">
-        <v>2295.37831639403</v>
+        <v>-2.60544229869128</v>
       </c>
       <c r="J9" t="n">
-        <v>2445.94945198473</v>
+        <v>2.77635286399028</v>
       </c>
       <c r="K9" t="n">
-        <v>3.388447477659</v>
+        <v>2.60544229869128</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.443474662483422</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.33061070880939</v>
+        <v>1.33061070879974</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>45266.6111111111</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" t="n">
         <v>615.23295</v>
@@ -2399,19 +2564,22 @@
         <v>0.0742687258801095</v>
       </c>
       <c r="G10" t="n">
-        <v>21.4097062585526</v>
+        <v>21.4097062580769</v>
       </c>
       <c r="H10" t="n">
         <v>63.18275</v>
       </c>
       <c r="I10" t="n">
-        <v>2.98405511927871</v>
+        <v>-0.00923424881936867</v>
       </c>
       <c r="J10" t="n">
-        <v>3.33938623369513</v>
+        <v>0.0103338316999215</v>
       </c>
       <c r="K10" t="n">
-        <v>0.523666652496055</v>
+        <v>0.00923424881936867</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-1.98573861579119</v>
       </c>
     </row>
     <row r="11">
@@ -2422,7 +2590,7 @@
         <v>45639.5510416667</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
         <v>526.36744</v>
@@ -2439,25 +2607,28 @@
       <c r="H11" t="n">
         <v>61.35475</v>
       </c>
-      <c r="I11" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J11" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K11" t="e">
-        <v>#NUM!</v>
+      <c r="I11" t="n">
+        <v>0.502258717663777</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.580860274637568</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.502258717663777</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-0.235928324153202</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.87799524404843</v>
+        <v>1.87799524404137</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>45331.4570601852</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" t="n">
         <v>504.21780864</v>
@@ -2469,30 +2640,33 @@
         <v>0.186952867332309</v>
       </c>
       <c r="G12" t="n">
-        <v>75.5083958708422</v>
+        <v>75.5083958696154</v>
       </c>
       <c r="H12" t="n">
         <v>56.771625</v>
       </c>
       <c r="I12" t="n">
-        <v>10.1233281358362</v>
+        <v>-0.0788577175808508</v>
       </c>
       <c r="J12" t="n">
-        <v>12.7446829017268</v>
+        <v>0.099277292154953</v>
       </c>
       <c r="K12" t="n">
-        <v>1.10532903433306</v>
+        <v>0.0788577175808508</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-1.0031500769787</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.71882276127153</v>
+        <v>1.71882276127598</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>45502.5288194444</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" t="n">
         <v>2747.582712</v>
@@ -2504,30 +2678,33 @@
         <v>0.142858205716412</v>
       </c>
       <c r="G13" t="n">
-        <v>52.3386795046643</v>
+        <v>52.3386795052</v>
       </c>
       <c r="H13" t="n">
         <v>74.3296666666667</v>
       </c>
       <c r="I13" t="n">
-        <v>39.1908375573378</v>
+        <v>-0.23328053058186</v>
       </c>
       <c r="J13" t="n">
-        <v>36.1951772221721</v>
+        <v>0.215449086397794</v>
       </c>
       <c r="K13" t="n">
-        <v>1.55865070740246</v>
+        <v>0.23328053058186</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-0.666655343178018</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2.09070650353942</v>
+        <v>2.09070650351727</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>45569.4864583333</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" t="n">
         <v>1103.890144</v>
@@ -2539,19 +2716,22 @@
         <v>0.267561157919519</v>
       </c>
       <c r="G14" t="n">
-        <v>123.227178179364</v>
+        <v>123.227178173077</v>
       </c>
       <c r="H14" t="n">
         <v>75.3264583333333</v>
       </c>
       <c r="I14" t="n">
-        <v>3.15911076136802</v>
+        <v>-0.0352189722211518</v>
       </c>
       <c r="J14" t="n">
-        <v>2.87051252902584</v>
+        <v>0.0320015690036934</v>
       </c>
       <c r="K14" t="n">
-        <v>0.457959446788</v>
+        <v>0.0352189722211518</v>
+      </c>
+      <c r="L14" t="n">
+        <v>-1.49482872815067</v>
       </c>
     </row>
   </sheetData>
@@ -2602,16 +2782,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.175260244808302</v>
+        <v>-0.175260244879322</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45684.6167824074</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" t="n">
         <v>450.504288</v>
@@ -2623,30 +2806,33 @@
         <v>0.106130731104437</v>
       </c>
       <c r="G2" t="n">
-        <v>0.66794354192741</v>
+        <v>0.667943541818182</v>
       </c>
       <c r="H2" t="n">
         <v>49.5106666666667</v>
       </c>
       <c r="I2" t="n">
-        <v>247.72983826695</v>
+        <v>-1.09548953548564</v>
       </c>
       <c r="J2" t="n">
-        <v>358.174369121744</v>
+        <v>1.58388781907339</v>
       </c>
       <c r="K2" t="n">
-        <v>2.55409450460832</v>
+        <v>1.09548953548564</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.199724418867947</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>-2.32800328872695</v>
+      <c r="A3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45590.4924768519</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="n">
         <v>505.046412</v>
@@ -2657,31 +2843,34 @@
       <c r="F3" t="n">
         <v>0.0301448591708373</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.00469890550310944</v>
+      <c r="G3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="H3" t="n">
         <v>67.9985833333333</v>
       </c>
       <c r="I3" t="n">
-        <v>204.408460187423</v>
+        <v>-0.256744343569899</v>
       </c>
       <c r="J3" t="n">
-        <v>210.092563052218</v>
+        <v>0.263883780252057</v>
       </c>
       <c r="K3" t="n">
-        <v>2.32241067933337</v>
+        <v>0.256744343569899</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-0.578587303086169</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-1.89676502842414</v>
+        <v>-1.9033044465218</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45296.6498842593</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="n">
         <v>637.0341</v>
@@ -2690,33 +2879,36 @@
         <v>1245.823</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0393744230845104</v>
+        <v>0.0392683187491522</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0126833790439043</v>
+        <v>0.0124938288823529</v>
       </c>
       <c r="H4" t="n">
-        <v>52.15875</v>
+        <v>51.9500869565217</v>
       </c>
       <c r="I4" t="n">
-        <v>201.152535994288</v>
+        <v>-0.328975995391074</v>
       </c>
       <c r="J4" t="n">
-        <v>276.378340533053</v>
+        <v>0.453880991435802</v>
       </c>
       <c r="K4" t="n">
-        <v>2.44150400485427</v>
+        <v>0.328975995391074</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.343058005156257</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.401820914597899</v>
+        <v>-0.401820914631298</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45502.5104166667</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="n">
         <v>718.57919</v>
@@ -2728,30 +2920,33 @@
         <v>0.0923400884564007</v>
       </c>
       <c r="G5" t="n">
-        <v>0.396441476915104</v>
+        <v>0.396441476884615</v>
       </c>
       <c r="H5" t="n">
         <v>76.43375</v>
       </c>
       <c r="I5" t="n">
-        <v>3.53500894211804</v>
+        <v>-0.0136009599337228</v>
       </c>
       <c r="J5" t="n">
-        <v>3.15399152008986</v>
+        <v>0.0121349939981598</v>
       </c>
       <c r="K5" t="n">
-        <v>0.498860521338119</v>
+        <v>0.0136009599337228</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1.91596043412947</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.07246895076231</v>
+        <v>2.07246895077545</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45279.5347222222</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="n">
         <v>811.21125</v>
@@ -2763,19 +2958,22 @@
         <v>0.386132065900496</v>
       </c>
       <c r="G6" t="n">
-        <v>118.159583308924</v>
+        <v>118.1595833125</v>
       </c>
       <c r="H6" t="n">
         <v>57.4105416666667</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0936575847248386</v>
+        <v>-0.00150684152821053</v>
       </c>
       <c r="J6" t="n">
-        <v>0.116487862981952</v>
+        <v>0.00187415413273145</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.933719321973188</v>
+        <v>0.00150684152821053</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-2.72719469506932</v>
       </c>
     </row>
   </sheetData>
@@ -2826,16 +3024,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.38306365667294</v>
+        <v>1.38306365666048</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45296.5511574074</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="n">
         <v>669.2205</v>
@@ -2847,19 +3048,22 @@
         <v>0.242294433819637</v>
       </c>
       <c r="G2" t="n">
-        <v>24.1581490633855</v>
+        <v>24.1581490626923</v>
       </c>
       <c r="H2" t="n">
         <v>57.088375</v>
       </c>
       <c r="I2" t="n">
-        <v>1.75024483467205</v>
+        <v>-0.0176697742192753</v>
       </c>
       <c r="J2" t="n">
-        <v>2.19012083047377</v>
+        <v>0.0221105869423432</v>
       </c>
       <c r="K2" t="n">
-        <v>0.340468075826607</v>
+        <v>0.0176697742192753</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1.65539972859101</v>
       </c>
     </row>
     <row r="3">
@@ -2868,7 +3072,7 @@
         <v>45684.5515046296</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
         <v>395.991756</v>
@@ -2886,16 +3090,19 @@
       <c r="K3" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="L3" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.24814091763682</v>
+        <v>1.24814091763677</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45590.450462963</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="n">
         <v>441.72498</v>
@@ -2907,30 +3114,33 @@
         <v>0.218316630467253</v>
       </c>
       <c r="G4" t="n">
-        <v>17.7068340734806</v>
+        <v>17.7068340734783</v>
       </c>
       <c r="H4" t="n">
         <v>69.407</v>
       </c>
       <c r="I4" t="n">
-        <v>5.62940675835463</v>
+        <v>-0.0512080464588985</v>
       </c>
       <c r="J4" t="n">
-        <v>5.64789055593064</v>
+        <v>0.0513761848091082</v>
       </c>
       <c r="K4" t="n">
-        <v>0.751886272424781</v>
+        <v>0.0512080464588985</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1.28923814954167</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.58978266162639</v>
+        <v>0.589782661626447</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45231.5222222222</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
         <v>744.31615</v>
@@ -2942,30 +3152,33 @@
         <v>0.13055244711888</v>
       </c>
       <c r="G5" t="n">
-        <v>3.88850499911487</v>
+        <v>3.88850499911538</v>
       </c>
       <c r="H5" t="n">
         <v>68.842375</v>
       </c>
       <c r="I5" t="n">
-        <v>3.67752525896693</v>
+        <v>-0.0200045800791511</v>
       </c>
       <c r="J5" t="n">
-        <v>3.72506216091881</v>
+        <v>0.0202631658657456</v>
       </c>
       <c r="K5" t="n">
-        <v>0.571133524310831</v>
+        <v>0.0200045800791511</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1.693292700604</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.7971276640854</v>
+        <v>2.79712766409306</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45279.41875</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
         <v>452.6567</v>
@@ -2977,30 +3190,33 @@
         <v>0.731386801864513</v>
       </c>
       <c r="G6" t="n">
-        <v>626.798089543104</v>
+        <v>626.798089554167</v>
       </c>
       <c r="H6" t="n">
         <v>60.1737083333333</v>
       </c>
       <c r="I6" t="n">
-        <v>0.586319530217814</v>
+        <v>-0.0178677652531963</v>
       </c>
       <c r="J6" t="n">
-        <v>0.692968790739059</v>
+        <v>0.0211178428187733</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.159286324284329</v>
+        <v>0.0178677652531963</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1.6753504469219</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.48911725947442</v>
+        <v>1.48911725947711</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>45569.4483796296</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
         <v>373.09719</v>
@@ -3012,19 +3228,22 @@
         <v>0.263452518093847</v>
       </c>
       <c r="G7" t="n">
-        <v>30.8402052313475</v>
+        <v>30.8402052315385</v>
       </c>
       <c r="H7" t="n">
         <v>76.0062916666667</v>
       </c>
       <c r="I7" t="n">
-        <v>22.5748045119931</v>
+        <v>-0.247807878923372</v>
       </c>
       <c r="J7" t="n">
-        <v>20.284117843621</v>
+        <v>0.222662580133929</v>
       </c>
       <c r="K7" t="n">
-        <v>1.30715612498201</v>
+        <v>0.247807878923372</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.652352762790092</v>
       </c>
     </row>
   </sheetData>
@@ -3075,16 +3294,19 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.13134059951358</v>
+        <v>1.13134059950346</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45660.5559027778</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
         <v>335.25396</v>
@@ -3096,30 +3318,33 @@
         <v>0.0500958747372041</v>
       </c>
       <c r="G2" t="n">
-        <v>13.531333546744</v>
+        <v>13.5313335464286</v>
       </c>
       <c r="H2" t="n">
         <v>50.861625</v>
       </c>
       <c r="I2" t="n">
-        <v>14.9622160341323</v>
+        <v>-0.0312310541765366</v>
       </c>
       <c r="J2" t="n">
-        <v>21.0761890923796</v>
+        <v>0.0439929220295616</v>
       </c>
       <c r="K2" t="n">
-        <v>1.32379208634261</v>
+        <v>0.0312310541765366</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1.35661719103134</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.27787649291049</v>
+        <v>2.27787649290113</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45296.6913194444</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
         <v>680.577033333333</v>
@@ -3131,30 +3356,33 @@
         <v>0.304619300450722</v>
       </c>
       <c r="G3" t="n">
-        <v>189.616660208254</v>
+        <v>189.616660204167</v>
       </c>
       <c r="H3" t="n">
         <v>52.2674583333333</v>
       </c>
       <c r="I3" t="n">
-        <v>3.24239418088936</v>
+        <v>-0.0411539936320003</v>
       </c>
       <c r="J3" t="n">
-        <v>4.44575197355207</v>
+        <v>0.0564275773400354</v>
       </c>
       <c r="K3" t="n">
-        <v>0.647945229950382</v>
+        <v>0.0411539936320003</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1.24850859531635</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.0158107754289</v>
+        <v>2.0158107753978</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45684.6496527778</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
         <v>365.76996</v>
@@ -3166,30 +3394,33 @@
         <v>0.201714359792356</v>
       </c>
       <c r="G4" t="n">
-        <v>103.707645726516</v>
+        <v>103.707645719091</v>
       </c>
       <c r="H4" t="n">
         <v>49.803125</v>
       </c>
       <c r="I4" t="n">
-        <v>17.1263820836176</v>
+        <v>-0.143943216564841</v>
       </c>
       <c r="J4" t="n">
-        <v>24.6242389760602</v>
+        <v>0.206960941684582</v>
       </c>
       <c r="K4" t="n">
-        <v>1.39136281729737</v>
+        <v>0.143943216564841</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-0.68411160822132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.97476751056966</v>
+        <v>1.97476751057974</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45590.5368055556</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
         <v>385.73862</v>
@@ -3201,30 +3432,33 @@
         <v>0.189070453385662</v>
       </c>
       <c r="G5" t="n">
-        <v>94.3555630543491</v>
+        <v>94.3555630565385</v>
       </c>
       <c r="H5" t="n">
         <v>67.770875</v>
       </c>
       <c r="I5" t="n">
-        <v>2.24948952918913</v>
+        <v>-0.0177213335487537</v>
       </c>
       <c r="J5" t="n">
-        <v>2.32142883577927</v>
+        <v>0.018288066770139</v>
       </c>
       <c r="K5" t="n">
-        <v>0.365755374755548</v>
+        <v>0.0177213335487537</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1.73783220132707</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.78483006309456</v>
+        <v>1.78483006308283</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45597.5128472222</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
         <v>366.03866</v>
@@ -3236,30 +3470,33 @@
         <v>0.140225032268246</v>
       </c>
       <c r="G6" t="n">
-        <v>60.9298435653969</v>
+        <v>60.92984356375</v>
       </c>
       <c r="H6" t="n">
         <v>68.7422083333333</v>
       </c>
       <c r="I6" t="n">
-        <v>5.98707457535708</v>
+        <v>-0.0349807385634102</v>
       </c>
       <c r="J6" t="n">
-        <v>6.07573352541785</v>
+        <v>0.0354987470689577</v>
       </c>
       <c r="K6" t="n">
-        <v>0.783598717959278</v>
+        <v>0.0349807385634102</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1.44978697513196</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.40231259910045</v>
+        <v>1.40231259910038</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>45618.5591435185</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" t="n">
         <v>2122.394256</v>
@@ -3271,30 +3508,33 @@
         <v>0.0767954910734997</v>
       </c>
       <c r="G7" t="n">
-        <v>25.2529779253888</v>
+        <v>25.2529779253846</v>
       </c>
       <c r="H7" t="n">
         <v>56.827625</v>
       </c>
       <c r="I7" t="n">
-        <v>324.265975905442</v>
+        <v>-1.03759020242025</v>
       </c>
       <c r="J7" t="n">
-        <v>407.818907929547</v>
+        <v>1.30494388764616</v>
       </c>
       <c r="K7" t="n">
-        <v>2.61046735733988</v>
+        <v>1.03759020242025</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.115591837490723</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.52348603915568</v>
+        <v>1.52348603914882</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>45266.6384259259</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
         <v>711.255675</v>
@@ -3306,30 +3546,33 @@
         <v>0.0929485828202428</v>
       </c>
       <c r="G8" t="n">
-        <v>33.3799774655278</v>
+        <v>33.379977465</v>
       </c>
       <c r="H8" t="n">
         <v>57.605125</v>
       </c>
       <c r="I8" t="n">
-        <v>1.74934976466679</v>
+        <v>-0.0067749825617793</v>
       </c>
       <c r="J8" t="n">
-        <v>2.16774731953429</v>
+        <v>0.00839537671929553</v>
       </c>
       <c r="K8" t="n">
-        <v>0.336008657881384</v>
+        <v>0.0067749825617793</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-2.07595981132575</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.19332484216351</v>
+        <v>1.19332484214905</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>45639.5956018518</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="n">
         <v>335.75364</v>
@@ -3339,7 +3582,7 @@
         <v>0.0552282276592525</v>
       </c>
       <c r="G9" t="n">
-        <v>15.6071944816737</v>
+        <v>15.6071944811538</v>
       </c>
       <c r="H9" t="n">
         <v>51.5931666666667</v>
@@ -3347,16 +3590,17 @@
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
+      <c r="L9"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.18247656019847</v>
+        <v>2.18247656018373</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>45331.5136574074</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" t="n">
         <v>464.2354962</v>
@@ -3368,30 +3612,33 @@
         <v>0.262140092531933</v>
       </c>
       <c r="G10" t="n">
-        <v>152.221697335934</v>
+        <v>152.221697330769</v>
       </c>
       <c r="H10" t="n">
         <v>55.680375</v>
       </c>
       <c r="I10" t="n">
-        <v>134.29547670046</v>
+        <v>-1.46684286203661</v>
       </c>
       <c r="J10" t="n">
-        <v>172.539893863929</v>
+        <v>1.88456765595585</v>
       </c>
       <c r="K10" t="n">
-        <v>2.23688952655034</v>
+        <v>1.46684286203661</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.275211733232091</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.82672653669575</v>
+        <v>1.82672653669478</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>45502.6175925926</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
         <v>703.29945</v>
@@ -3403,30 +3650,33 @@
         <v>0.149697122890749</v>
       </c>
       <c r="G11" t="n">
-        <v>67.1006205701499</v>
+        <v>67.10062057</v>
       </c>
       <c r="H11" t="n">
         <v>77.6787083333333</v>
       </c>
       <c r="I11" t="n">
-        <v>18.435644843617</v>
+        <v>-0.114990124655214</v>
       </c>
       <c r="J11" t="n">
-        <v>16.1197447508915</v>
+        <v>0.100544975455905</v>
       </c>
       <c r="K11" t="n">
-        <v>1.20735816066033</v>
+        <v>0.114990124655214</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-0.99763962756647</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.99011538979048</v>
+        <v>1.99011538980078</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>45569.5574074074</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
         <v>403.8474</v>
@@ -3438,19 +3688,22 @@
         <v>0.193682525546869</v>
       </c>
       <c r="G12" t="n">
-        <v>97.7496902311427</v>
+        <v>97.7496902334615</v>
       </c>
       <c r="H12" t="n">
         <v>76.7826666666667</v>
       </c>
       <c r="I12" t="n">
-        <v>3.52886405062264</v>
+        <v>-0.0284783042348395</v>
       </c>
       <c r="J12" t="n">
-        <v>3.13101582511279</v>
+        <v>0.0252676271889608</v>
       </c>
       <c r="K12" t="n">
-        <v>0.495685262679768</v>
+        <v>0.0284783042348395</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-1.59743553952547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating DOC, DIC, gas sampling
</commit_message>
<xml_diff>
--- a/04_Output/rC_k600.xlsx
+++ b/04_Output/rC_k600.xlsx
@@ -792,7 +792,7 @@
         <v>638.458466666667</v>
       </c>
       <c r="E2" t="n">
-        <v>3992.646</v>
+        <v>8509.227</v>
       </c>
       <c r="F2" t="n">
         <v>0.195852248068133</v>
@@ -804,16 +804,16 @@
         <v>53.7677083333333</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.0470281004199628</v>
+        <v>-0.0191543497943117</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0626672954135077</v>
+        <v>0.0255241288994157</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0470281004199628</v>
+        <v>0.0191543497943117</v>
       </c>
       <c r="L2" t="n">
-        <v>-1.20295904811693</v>
+        <v>-1.59304907081334</v>
       </c>
     </row>
     <row r="3">
@@ -833,25 +833,25 @@
         <v>1052.144</v>
       </c>
       <c r="F3" t="n">
-        <v>0.277576481764534</v>
+        <v>0.274027142180158</v>
       </c>
       <c r="G3" t="n">
         <v>82.9004011751482</v>
       </c>
       <c r="H3" t="n">
-        <v>51.2003333333333</v>
+        <v>52.302625</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.371734272889384</v>
+        <v>-0.377725427512456</v>
       </c>
       <c r="J3" t="n">
-        <v>0.520198524602315</v>
+        <v>0.517554434954518</v>
       </c>
       <c r="K3" t="n">
-        <v>0.371734272889384</v>
+        <v>0.377725427512456</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.283830883893283</v>
+        <v>-0.286043965567491</v>
       </c>
     </row>
     <row r="4">
@@ -982,7 +982,7 @@
         <v>743.7952</v>
       </c>
       <c r="E7" t="n">
-        <v>3992.646</v>
+        <v>8757.557</v>
       </c>
       <c r="F7" t="n">
         <v>0.508260069853473</v>
@@ -994,16 +994,16 @@
         <v>57.950125</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.541345524111269</v>
+        <v>-0.141260996271992</v>
       </c>
       <c r="J7" t="n">
-        <v>0.666557303146162</v>
+        <v>0.173934288769413</v>
       </c>
       <c r="K7" t="n">
-        <v>0.541345524111269</v>
+        <v>0.141260996271992</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.176162508860153</v>
+        <v>-0.759614794331786</v>
       </c>
     </row>
     <row r="8">
@@ -1020,7 +1020,7 @@
         <v>801.7695</v>
       </c>
       <c r="E8" t="n">
-        <v>4010.916</v>
+        <v>4026.08</v>
       </c>
       <c r="F8" t="n">
         <v>0.292017862477283</v>
@@ -1032,16 +1032,16 @@
         <v>76.3831666666667</v>
       </c>
       <c r="I8" t="n">
-        <v>1.39006128539709</v>
+        <v>1.40185787623314</v>
       </c>
       <c r="J8" t="n">
-        <v>1.24132745720325</v>
+        <v>1.2518618359821</v>
       </c>
       <c r="K8" t="n">
-        <v>1.39006128539709</v>
+        <v>1.40185787623314</v>
       </c>
       <c r="L8" t="n">
-        <v>0.093886361754324</v>
+        <v>0.0975563998155705</v>
       </c>
     </row>
     <row r="9">
@@ -1189,25 +1189,25 @@
         <v>5860.433</v>
       </c>
       <c r="F3" t="n">
-        <v>0.524586113304458</v>
+        <v>0.514403686709471</v>
       </c>
       <c r="G3" t="n">
         <v>123.942374733896</v>
       </c>
       <c r="H3" t="n">
-        <v>51.4724285714286</v>
+        <v>52.1867083333333</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0147276608619273</v>
+        <v>-0.0148789334135516</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0205028926262647</v>
+        <v>0.0204362129975192</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0147276608619273</v>
+        <v>0.0148789334135516</v>
       </c>
       <c r="L3" t="n">
-        <v>-1.68818486270022</v>
+        <v>-1.6895995795088</v>
       </c>
     </row>
     <row r="4">
@@ -1504,28 +1504,28 @@
         <v>560.080524</v>
       </c>
       <c r="E3" t="n">
-        <v>3223.928</v>
+        <v>3799.521</v>
       </c>
       <c r="F3" t="n">
-        <v>0.221457401795922</v>
+        <v>0.216853459021603</v>
       </c>
       <c r="G3" t="n">
         <v>139.818789841654</v>
       </c>
       <c r="H3" t="n">
-        <v>53.0998181818182</v>
+        <v>53.521625</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.16229705182373</v>
+        <v>-0.1288164418135</v>
       </c>
       <c r="J3" t="n">
-        <v>0.21903335975322</v>
+        <v>0.17242135645319</v>
       </c>
       <c r="K3" t="n">
-        <v>0.16229705182373</v>
+        <v>0.1288164418135</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.65948973514438</v>
+        <v>-0.76340894259866</v>
       </c>
     </row>
     <row r="4">
@@ -2053,25 +2053,25 @@
         <v>4929.498</v>
       </c>
       <c r="F3" t="n">
-        <v>0.523142070899526</v>
+        <v>0.519697920654582</v>
       </c>
       <c r="G3" t="n">
         <v>23.057974912815</v>
       </c>
       <c r="H3" t="n">
-        <v>52.7025454545455</v>
+        <v>53.17225</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.196505893268312</v>
+        <v>-0.197842978098901</v>
       </c>
       <c r="J3" t="n">
-        <v>0.26721608984759</v>
+        <v>0.266638686605334</v>
       </c>
       <c r="K3" t="n">
-        <v>0.196505893268312</v>
+        <v>0.197842978098901</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.573137395292139</v>
+        <v>-0.574076838566927</v>
       </c>
     </row>
     <row r="4">
@@ -2254,7 +2254,7 @@
         <v>350.63274</v>
       </c>
       <c r="E2" t="n">
-        <v>7013.68</v>
+        <v>12349.884</v>
       </c>
       <c r="F2" t="n">
         <v>0.128743864480736</v>
@@ -2266,16 +2266,16 @@
         <v>60.6108333333333</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.0457362341132933</v>
+        <v>-0.0248130778879441</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0536290117969964</v>
+        <v>0.0290951118423101</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0457362341132933</v>
+        <v>0.0248130778879441</v>
       </c>
       <c r="L2" t="n">
-        <v>-1.2706002055554</v>
+        <v>-1.53617996902892</v>
       </c>
     </row>
     <row r="3">
@@ -2333,25 +2333,25 @@
         <v>7013.68</v>
       </c>
       <c r="F4" t="n">
-        <v>0.399089827931722</v>
+        <v>0.391295963011507</v>
       </c>
       <c r="G4" t="n">
         <v>134.461029345514</v>
       </c>
       <c r="H4" t="n">
-        <v>52.6218666666667</v>
+        <v>53.2519166666667</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.0142344689232062</v>
+        <v>-0.0143649998659057</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0193832495193451</v>
+        <v>0.0193268918419151</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0142344689232062</v>
+        <v>0.0143649998659057</v>
       </c>
       <c r="L4" t="n">
-        <v>-1.71257341355879</v>
+        <v>-1.71383798375942</v>
       </c>
     </row>
     <row r="5">
@@ -2803,7 +2803,7 @@
         <v>1244.816</v>
       </c>
       <c r="F2" t="n">
-        <v>0.306130731104437</v>
+        <v>0.303866762065075</v>
       </c>
       <c r="G2" t="n">
         <v>37.5419690591882</v>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.20217527191572</v>
+        <v>1.2025711866528</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>45296.6498842593</v>
@@ -2879,25 +2879,25 @@
         <v>1245.823</v>
       </c>
       <c r="F4" t="n">
-        <v>0.239311089488986</v>
+        <v>0.23937442308451</v>
       </c>
       <c r="G4" t="n">
-        <v>15.9285143794493</v>
+        <v>15.943041869971</v>
       </c>
       <c r="H4" t="n">
-        <v>52.0356923076923</v>
+        <v>52.15875</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.329406983852389</v>
+        <v>-0.330011044031721</v>
       </c>
       <c r="J4" t="n">
-        <v>0.453691558065658</v>
+        <v>0.453426571314305</v>
       </c>
       <c r="K4" t="n">
-        <v>0.329406983852389</v>
+        <v>0.330011044031721</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.343239301667664</v>
+        <v>-0.343493033311727</v>
       </c>
     </row>
     <row r="5">
@@ -2914,7 +2914,7 @@
         <v>718.57919</v>
       </c>
       <c r="E5" t="n">
-        <v>20938.13</v>
+        <v>1573.128</v>
       </c>
       <c r="F5" t="n">
         <v>0.292340088456401</v>
@@ -2926,16 +2926,16 @@
         <v>76.43375</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0136009599337228</v>
+        <v>-0.493194293879235</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0121349939981598</v>
+        <v>0.440035837567019</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0136009599337228</v>
+        <v>0.493194293879235</v>
       </c>
       <c r="L5" t="n">
-        <v>-1.91596043412947</v>
+        <v>-0.356511952096092</v>
       </c>
     </row>
     <row r="6">
@@ -3067,7 +3067,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3"/>
+      <c r="A3" t="n">
+        <v>1.92653479913752</v>
+      </c>
       <c r="B3" s="1" t="n">
         <v>45684.5515046296</v>
       </c>
@@ -3077,21 +3079,29 @@
       <c r="D3" t="n">
         <v>395.991756</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L3" t="e">
-        <v>#NUM!</v>
+      <c r="E3" t="n">
+        <v>7475.905</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.327860796281033</v>
+      </c>
+      <c r="G3" t="n">
+        <v>84.4373897169224</v>
+      </c>
+      <c r="H3" t="n">
+        <v>52.7094583333333</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.552638322840444</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.751239608585646</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.552638322840444</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-0.124221522263913</v>
       </c>
     </row>
     <row r="4">
@@ -3312,7 +3322,7 @@
         <v>335.25396</v>
       </c>
       <c r="E2" t="n">
-        <v>3393.52</v>
+        <v>3903.276</v>
       </c>
       <c r="F2" t="n">
         <v>0.0500958747372041</v>
@@ -3324,16 +3334,16 @@
         <v>50.861625</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.0312310541765366</v>
+        <v>-0.0265712094335327</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0439929220295616</v>
+        <v>0.037428936539669</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0312310541765366</v>
+        <v>0.0265712094335327</v>
       </c>
       <c r="L2" t="n">
-        <v>-1.35661719103134</v>
+        <v>-1.42679251222607</v>
       </c>
     </row>
     <row r="3">
@@ -3391,25 +3401,25 @@
         <v>3393.52</v>
       </c>
       <c r="F4" t="n">
-        <v>0.201714359792356</v>
+        <v>0.196666010534818</v>
       </c>
       <c r="G4" t="n">
         <v>85.0746956266847</v>
       </c>
       <c r="H4" t="n">
-        <v>49.803125</v>
+        <v>50.6177916666667</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.143943216564841</v>
+        <v>-0.145662173571032</v>
       </c>
       <c r="J4" t="n">
-        <v>0.206960941684582</v>
+        <v>0.206182707231445</v>
       </c>
       <c r="K4" t="n">
-        <v>0.143943216564841</v>
+        <v>0.145662173571032</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.68411160822132</v>
+        <v>-0.685747762277013</v>
       </c>
     </row>
     <row r="5">

</xml_diff>